<commit_message>
Winder working to a schedule and added Steps per Day functionality
</commit_message>
<xml_diff>
--- a/ESP32.xlsx
+++ b/ESP32.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dyoud/projects/smart-watch-winder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674B5E53-4DBE-1D4A-91FF-E9F07750AD4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288E938F-A3F5-E646-9F2E-923BFF8DA056}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34580" yWindow="120" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="1440" windowWidth="28800" windowHeight="16140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="ESP32_Pinout" sheetId="2" r:id="rId2"/>
     <sheet name="ArduinoCam Pinout" sheetId="3" r:id="rId3"/>
+    <sheet name="Turns per day" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ESP32_Pinout!$A$1:$T$57</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="331">
   <si>
     <t>ESP32</t>
   </si>
@@ -969,12 +971,81 @@
   <si>
     <t>Winder_4</t>
   </si>
+  <si>
+    <t>STEPS_PER_REVOLUTION</t>
+  </si>
+  <si>
+    <t>Param</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>WINDER_DELAY_CYCLES</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>Target TPD</t>
+  </si>
+  <si>
+    <t>WINDER_ROTATIONS_PER_CYCLE</t>
+  </si>
+  <si>
+    <t>turns</t>
+  </si>
+  <si>
+    <t>WIND_BOTH_DIRECTIONS</t>
+  </si>
+  <si>
+    <t>Suggested settings</t>
+  </si>
+  <si>
+    <t>ms per minute</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>intervals per day</t>
+  </si>
+  <si>
+    <t>Intervals per day</t>
+  </si>
+  <si>
+    <t>time per interval</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>time per rotation</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>ms per day</t>
+  </si>
+  <si>
+    <t>once every 15min</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1037,6 +1108,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1076,7 +1163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1114,6 +1201,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1431,7 +1522,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1620,7 +1711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="O27" sqref="O27:O40"/>
     </sheetView>
   </sheetViews>
@@ -3199,4 +3290,156 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4EAACE0-BA9E-C141-BD01-1945B6E3105A}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19">
+      <c r="A2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2">
+        <v>2048</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I2" s="26">
+        <f>D7*D4*IF(D5,2,1)</f>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D3">
+        <v>900000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>316</v>
+      </c>
+      <c r="C4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D6">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D7" s="28">
+        <f>D10/D3</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>324</v>
+      </c>
+      <c r="C8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8">
+        <f>D4*D9</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>326</v>
+      </c>
+      <c r="C9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="27">
+        <v>86400000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>